<commit_message>
Updated the Project Schedule and Forecast -> Facebook post template.
</commit_message>
<xml_diff>
--- a/docs/Project-Schedule.xlsx
+++ b/docs/Project-Schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="172">
   <si>
     <t>MODULE</t>
   </si>
@@ -628,6 +628,12 @@
   </si>
   <si>
     <t>Transactions Client</t>
+  </si>
+  <si>
+    <t>HOURS</t>
+  </si>
+  <si>
+    <t>DAYS</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H571"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B172" sqref="B172"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I176" sqref="I176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,9 +1101,7 @@
       <c r="G1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -1327,7 +1331,9 @@
       <c r="F15" s="5">
         <v>8</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
@@ -1388,18 +1394,20 @@
     </row>
     <row r="19" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="13">
         <v>12</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
@@ -1430,8 +1438,12 @@
         <v>8</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="F21" s="13">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
@@ -1445,7 +1457,9 @@
         <v>16</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="F22" s="13">
+        <v>16</v>
+      </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1460,7 +1474,9 @@
         <v>24</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="13">
+        <v>24</v>
+      </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1476,7 +1492,9 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
@@ -1507,8 +1525,12 @@
         <v>8</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="3"/>
+      <c r="F26" s="5">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
@@ -1522,7 +1544,9 @@
         <v>16</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="5">
+        <v>16</v>
+      </c>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1537,7 +1561,9 @@
         <v>24</v>
       </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="5">
+        <v>24</v>
+      </c>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1553,7 +1579,9 @@
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="30" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
@@ -1582,7 +1610,9 @@
         <v>8</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="F31" s="5">
+        <v>8</v>
+      </c>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1597,7 +1627,9 @@
         <v>24</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="F32" s="5">
+        <v>12</v>
+      </c>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1612,7 +1644,9 @@
         <v>16</v>
       </c>
       <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="F33" s="5">
+        <v>8</v>
+      </c>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1627,7 +1661,9 @@
         <v>16</v>
       </c>
       <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+      <c r="F34" s="5">
+        <v>8</v>
+      </c>
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1642,7 +1678,9 @@
         <v>16</v>
       </c>
       <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+      <c r="F35" s="5">
+        <v>8</v>
+      </c>
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1657,7 +1695,9 @@
         <v>8</v>
       </c>
       <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="5">
+        <v>4</v>
+      </c>
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1672,7 +1712,9 @@
         <v>16</v>
       </c>
       <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="F37" s="5">
+        <v>8</v>
+      </c>
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1687,7 +1729,9 @@
         <v>16</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="F38" s="5">
+        <v>8</v>
+      </c>
       <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1702,7 +1746,9 @@
         <v>16</v>
       </c>
       <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
+      <c r="F39" s="5">
+        <v>8</v>
+      </c>
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1717,7 +1763,9 @@
         <v>16</v>
       </c>
       <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
+      <c r="F40" s="5">
+        <v>8</v>
+      </c>
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1915,17 +1963,19 @@
     </row>
     <row r="52" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="3">
         <v>24</v>
       </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3">
+        <v>12</v>
+      </c>
       <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1960,7 +2010,9 @@
       <c r="F54" s="5">
         <v>8</v>
       </c>
-      <c r="G54" s="5"/>
+      <c r="G54" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="55" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8"/>
@@ -2009,7 +2061,9 @@
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
+      <c r="G57" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="58" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
@@ -2126,7 +2180,9 @@
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
+      <c r="G64" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="65" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
@@ -2141,7 +2197,9 @@
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
+      <c r="G65" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="66" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
@@ -2156,7 +2214,9 @@
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
+      <c r="G66" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="67" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="10"/>
@@ -2239,7 +2299,9 @@
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
+      <c r="G71" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="72" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8"/>
@@ -2305,7 +2367,9 @@
       </c>
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
-      <c r="G75" s="3"/>
+      <c r="G75" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="76" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8"/>
@@ -2337,7 +2401,9 @@
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
-      <c r="G77" s="3"/>
+      <c r="G77" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="78" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="8"/>
@@ -2369,7 +2435,9 @@
       </c>
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
-      <c r="G79" s="3"/>
+      <c r="G79" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="80" spans="1:7" s="4" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="8"/>
@@ -2401,7 +2469,9 @@
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
+      <c r="G81" s="5">
+        <v>12</v>
+      </c>
     </row>
     <row r="82" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="8"/>
@@ -2432,8 +2502,12 @@
         <v>8</v>
       </c>
       <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
+      <c r="F83" s="5">
+        <v>8</v>
+      </c>
+      <c r="G83" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="84" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="8"/>
@@ -2482,7 +2556,9 @@
       </c>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
+      <c r="G86" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="87" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="8"/>
@@ -2565,22 +2641,28 @@
       </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
-      <c r="G91" s="5"/>
+      <c r="G91" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="92" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="8"/>
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C92" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D92" s="5">
+      <c r="D92" s="3">
         <v>24</v>
       </c>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="E92" s="3">
+        <v>12</v>
+      </c>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="93" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="8"/>
@@ -2611,22 +2693,30 @@
         <v>8</v>
       </c>
       <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
+      <c r="F94" s="5">
+        <v>8</v>
+      </c>
+      <c r="G94" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="95" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="8"/>
-      <c r="B95" s="11" t="s">
+      <c r="B95" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D95" s="5">
+      <c r="D95" s="3">
         <v>16</v>
       </c>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
+      <c r="E95" s="3">
+        <v>8</v>
+      </c>
+      <c r="F95" s="3">
+        <v>8</v>
+      </c>
       <c r="G95" s="5"/>
     </row>
     <row r="96" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2641,10 +2731,10 @@
         <v>16</v>
       </c>
       <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5">
+      <c r="F96" s="5">
         <v>16</v>
       </c>
+      <c r="G96" s="5"/>
     </row>
     <row r="97" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="8"/>
@@ -2659,7 +2749,9 @@
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
+      <c r="G97" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="98" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="8"/>
@@ -2706,7 +2798,9 @@
       <c r="D100" s="3">
         <v>24</v>
       </c>
-      <c r="E100" s="3"/>
+      <c r="E100" s="3">
+        <v>12</v>
+      </c>
       <c r="F100" s="3">
         <v>12</v>
       </c>
@@ -2778,7 +2872,9 @@
       <c r="F104" s="5">
         <v>8</v>
       </c>
-      <c r="G104" s="5"/>
+      <c r="G104" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="105" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="8"/>
@@ -2844,7 +2940,9 @@
       </c>
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
-      <c r="G108" s="5"/>
+      <c r="G108" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="109" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="8"/>
@@ -2878,7 +2976,9 @@
       <c r="F110" s="5">
         <v>16</v>
       </c>
-      <c r="G110" s="5"/>
+      <c r="G110" s="5">
+        <v>16</v>
+      </c>
     </row>
     <row r="111" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="8"/>
@@ -2961,7 +3061,9 @@
       </c>
       <c r="E115" s="5"/>
       <c r="F115" s="5"/>
-      <c r="G115" s="5"/>
+      <c r="G115" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="116" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="8"/>
@@ -2992,7 +3094,9 @@
         <v>8</v>
       </c>
       <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
+      <c r="F117" s="5">
+        <v>8</v>
+      </c>
       <c r="G117" s="5"/>
     </row>
     <row r="118" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3007,7 +3111,9 @@
         <v>12</v>
       </c>
       <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
+      <c r="F118" s="5">
+        <v>12</v>
+      </c>
       <c r="G118" s="5"/>
     </row>
     <row r="119" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3023,7 +3129,9 @@
       </c>
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
-      <c r="G119" s="5"/>
+      <c r="G119" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="120" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="8"/>
@@ -3037,7 +3145,9 @@
         <v>12</v>
       </c>
       <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
+      <c r="F120" s="5">
+        <v>12</v>
+      </c>
       <c r="G120" s="5"/>
     </row>
     <row r="121" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3053,7 +3163,9 @@
       </c>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
+      <c r="G121" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="122" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="8"/>
@@ -3067,7 +3179,9 @@
         <v>12</v>
       </c>
       <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
+      <c r="F122" s="5">
+        <v>12</v>
+      </c>
       <c r="G122" s="5"/>
     </row>
     <row r="123" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3083,7 +3197,9 @@
       </c>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
-      <c r="G123" s="5"/>
+      <c r="G123" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="124" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="8"/>
@@ -3097,7 +3213,9 @@
         <v>12</v>
       </c>
       <c r="E124" s="5"/>
-      <c r="F124" s="5"/>
+      <c r="F124" s="5">
+        <v>12</v>
+      </c>
       <c r="G124" s="5"/>
     </row>
     <row r="125" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3113,7 +3231,9 @@
       </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
-      <c r="G125" s="5"/>
+      <c r="G125" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="126" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="8"/>
@@ -3127,7 +3247,9 @@
         <v>12</v>
       </c>
       <c r="E126" s="5"/>
-      <c r="F126" s="5"/>
+      <c r="F126" s="5">
+        <v>12</v>
+      </c>
       <c r="G126" s="5"/>
     </row>
     <row r="127" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3143,7 +3265,9 @@
       </c>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
-      <c r="G127" s="5"/>
+      <c r="G127" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="128" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="8"/>
@@ -3157,7 +3281,9 @@
         <v>16</v>
       </c>
       <c r="E128" s="5"/>
-      <c r="F128" s="5"/>
+      <c r="F128" s="5">
+        <v>12</v>
+      </c>
       <c r="G128" s="5"/>
     </row>
     <row r="129" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3173,7 +3299,9 @@
       </c>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
-      <c r="G129" s="5"/>
+      <c r="G129" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="130" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="8"/>
@@ -3204,8 +3332,12 @@
         <v>8</v>
       </c>
       <c r="E131" s="5"/>
-      <c r="F131" s="5"/>
-      <c r="G131" s="5"/>
+      <c r="F131" s="5">
+        <v>8</v>
+      </c>
+      <c r="G131" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="132" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="8"/>
@@ -3219,7 +3351,9 @@
         <v>16</v>
       </c>
       <c r="E132" s="5"/>
-      <c r="F132" s="5"/>
+      <c r="F132" s="5">
+        <v>16</v>
+      </c>
       <c r="G132" s="5"/>
     </row>
     <row r="133" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3235,7 +3369,9 @@
       </c>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
-      <c r="G133" s="5"/>
+      <c r="G133" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="134" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="8"/>
@@ -3249,7 +3385,9 @@
         <v>16</v>
       </c>
       <c r="E134" s="5"/>
-      <c r="F134" s="5"/>
+      <c r="F134" s="5">
+        <v>16</v>
+      </c>
       <c r="G134" s="5"/>
     </row>
     <row r="135" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3265,7 +3403,9 @@
       </c>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
-      <c r="G135" s="5"/>
+      <c r="G135" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="136" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="8"/>
@@ -3279,7 +3419,9 @@
         <v>12</v>
       </c>
       <c r="E136" s="5"/>
-      <c r="F136" s="5"/>
+      <c r="F136" s="5">
+        <v>12</v>
+      </c>
       <c r="G136" s="5"/>
     </row>
     <row r="137" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3295,7 +3437,9 @@
       </c>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
-      <c r="G137" s="5"/>
+      <c r="G137" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="138" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="8"/>
@@ -3309,7 +3453,9 @@
         <v>12</v>
       </c>
       <c r="E138" s="5"/>
-      <c r="F138" s="5"/>
+      <c r="F138" s="5">
+        <v>12</v>
+      </c>
       <c r="G138" s="5"/>
     </row>
     <row r="139" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3325,7 +3471,9 @@
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
-      <c r="G139" s="5"/>
+      <c r="G139" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="140" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="8"/>
@@ -3339,7 +3487,9 @@
         <v>12</v>
       </c>
       <c r="E140" s="5"/>
-      <c r="F140" s="5"/>
+      <c r="F140" s="5">
+        <v>12</v>
+      </c>
       <c r="G140" s="5"/>
     </row>
     <row r="141" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3355,7 +3505,9 @@
       </c>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
-      <c r="G141" s="5"/>
+      <c r="G141" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="142" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="8"/>
@@ -3369,7 +3521,9 @@
         <v>12</v>
       </c>
       <c r="E142" s="5"/>
-      <c r="F142" s="5"/>
+      <c r="F142" s="5">
+        <v>12</v>
+      </c>
       <c r="G142" s="5"/>
     </row>
     <row r="143" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3385,7 +3539,9 @@
       </c>
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
-      <c r="G143" s="5"/>
+      <c r="G143" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="144" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="8"/>
@@ -3399,7 +3555,9 @@
         <v>16</v>
       </c>
       <c r="E144" s="5"/>
-      <c r="F144" s="5"/>
+      <c r="F144" s="5">
+        <v>16</v>
+      </c>
       <c r="G144" s="5"/>
     </row>
     <row r="145" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3415,7 +3573,9 @@
       </c>
       <c r="E145" s="5"/>
       <c r="F145" s="5"/>
-      <c r="G145" s="5"/>
+      <c r="G145" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="146" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="8"/>
@@ -3429,7 +3589,9 @@
         <v>16</v>
       </c>
       <c r="E146" s="5"/>
-      <c r="F146" s="5"/>
+      <c r="F146" s="5">
+        <v>16</v>
+      </c>
       <c r="G146" s="5"/>
     </row>
     <row r="147" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3445,7 +3607,9 @@
       </c>
       <c r="E147" s="5"/>
       <c r="F147" s="5"/>
-      <c r="G147" s="5"/>
+      <c r="G147" s="5">
+        <v>24</v>
+      </c>
     </row>
     <row r="148" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="8"/>
@@ -3464,16 +3628,22 @@
       <c r="A149" s="8">
         <v>24</v>
       </c>
-      <c r="B149" s="11" t="s">
+      <c r="B149" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D149" s="5">
-        <v>8</v>
-      </c>
-      <c r="G149" s="5"/>
+      <c r="D149" s="3">
+        <v>8</v>
+      </c>
+      <c r="E149" s="4"/>
+      <c r="F149" s="3">
+        <v>8</v>
+      </c>
+      <c r="G149" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="150" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="8"/>
@@ -3486,6 +3656,10 @@
       <c r="D150" s="5">
         <v>16</v>
       </c>
+      <c r="E150" s="5">
+        <v>16</v>
+      </c>
+      <c r="F150" s="5"/>
       <c r="G150" s="5"/>
     </row>
     <row r="151" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3499,20 +3673,29 @@
       <c r="D151" s="5">
         <v>40</v>
       </c>
+      <c r="F151" s="5">
+        <v>40</v>
+      </c>
       <c r="G151" s="5"/>
     </row>
     <row r="152" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="8"/>
-      <c r="B152" s="11" t="s">
+      <c r="B152" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C152" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D152" s="5">
+      <c r="D152" s="3">
         <v>48</v>
       </c>
-      <c r="G152" s="5"/>
+      <c r="E152" s="3">
+        <v>12</v>
+      </c>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3">
+        <v>36</v>
+      </c>
     </row>
     <row r="153" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="8"/>
@@ -3525,20 +3708,29 @@
       <c r="D153" s="5">
         <v>16</v>
       </c>
+      <c r="F153" s="5">
+        <v>16</v>
+      </c>
       <c r="G153" s="5"/>
     </row>
     <row r="154" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="8"/>
-      <c r="B154" s="11" t="s">
+      <c r="B154" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="C154" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D154" s="5">
+      <c r="D154" s="3">
         <v>24</v>
       </c>
-      <c r="G154" s="5"/>
+      <c r="E154" s="3">
+        <v>8</v>
+      </c>
+      <c r="F154" s="4"/>
+      <c r="G154" s="3">
+        <v>16</v>
+      </c>
     </row>
     <row r="155" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="8"/>
@@ -3642,7 +3834,7 @@
       <c r="F160" s="5"/>
       <c r="G160" s="5"/>
     </row>
-    <row r="161" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="8"/>
       <c r="B161" s="11" t="s">
         <v>73</v>
@@ -3657,7 +3849,7 @@
       <c r="F161" s="5"/>
       <c r="G161" s="5"/>
     </row>
-    <row r="162" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="8"/>
       <c r="B162" s="11" t="s">
         <v>74</v>
@@ -3672,7 +3864,7 @@
       <c r="F162" s="5"/>
       <c r="G162" s="5"/>
     </row>
-    <row r="163" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="8"/>
       <c r="B163" s="11" t="s">
         <v>75</v>
@@ -3687,7 +3879,7 @@
       <c r="F163" s="5"/>
       <c r="G163" s="5"/>
     </row>
-    <row r="164" spans="1:7" s="6" customFormat="1" ht="70.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" s="6" customFormat="1" ht="70.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="8"/>
       <c r="B164" s="12" t="s">
         <v>95</v>
@@ -3702,7 +3894,7 @@
       <c r="F164" s="5"/>
       <c r="G164" s="5"/>
     </row>
-    <row r="165" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="8">
         <v>27</v>
       </c>
@@ -3716,10 +3908,12 @@
         <v>4</v>
       </c>
       <c r="E165" s="5"/>
-      <c r="F165" s="5"/>
+      <c r="F165" s="5">
+        <v>2</v>
+      </c>
       <c r="G165" s="5"/>
     </row>
-    <row r="166" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="8"/>
       <c r="B166" s="11" t="s">
         <v>78</v>
@@ -3731,10 +3925,12 @@
         <v>4</v>
       </c>
       <c r="E166" s="5"/>
-      <c r="F166" s="5"/>
+      <c r="F166" s="5">
+        <v>2</v>
+      </c>
       <c r="G166" s="5"/>
     </row>
-    <row r="167" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="8"/>
       <c r="B167" s="11" t="s">
         <v>79</v>
@@ -3746,10 +3942,12 @@
         <v>4</v>
       </c>
       <c r="E167" s="5"/>
-      <c r="F167" s="5"/>
+      <c r="F167" s="5">
+        <v>2</v>
+      </c>
       <c r="G167" s="5"/>
     </row>
-    <row r="168" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="8"/>
       <c r="B168" s="11" t="s">
         <v>80</v>
@@ -3761,10 +3959,12 @@
         <v>4</v>
       </c>
       <c r="E168" s="5"/>
-      <c r="F168" s="5"/>
+      <c r="F168" s="5">
+        <v>2</v>
+      </c>
       <c r="G168" s="5"/>
     </row>
-    <row r="169" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="8"/>
       <c r="B169" s="11" t="s">
         <v>81</v>
@@ -3776,10 +3976,12 @@
         <v>4</v>
       </c>
       <c r="E169" s="5"/>
-      <c r="F169" s="5"/>
+      <c r="F169" s="5">
+        <v>2</v>
+      </c>
       <c r="G169" s="5"/>
     </row>
-    <row r="170" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="8"/>
       <c r="B170" s="11" t="s">
         <v>82</v>
@@ -3791,10 +3993,12 @@
         <v>4</v>
       </c>
       <c r="E170" s="5"/>
-      <c r="F170" s="5"/>
+      <c r="F170" s="5">
+        <v>2</v>
+      </c>
       <c r="G170" s="5"/>
     </row>
-    <row r="171" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="8"/>
       <c r="B171" s="11" t="s">
         <v>83</v>
@@ -3806,10 +4010,12 @@
         <v>4</v>
       </c>
       <c r="E171" s="5"/>
-      <c r="F171" s="5"/>
+      <c r="F171" s="5">
+        <v>2</v>
+      </c>
       <c r="G171" s="5"/>
     </row>
-    <row r="172" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="8"/>
       <c r="B172" s="11" t="s">
         <v>84</v>
@@ -3821,10 +4027,12 @@
         <v>4</v>
       </c>
       <c r="E172" s="5"/>
-      <c r="F172" s="5"/>
+      <c r="F172" s="5">
+        <v>2</v>
+      </c>
       <c r="G172" s="5"/>
     </row>
-    <row r="173" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="8"/>
       <c r="B173" s="11" t="s">
         <v>85</v>
@@ -3836,10 +4044,12 @@
         <v>4</v>
       </c>
       <c r="E173" s="5"/>
-      <c r="F173" s="5"/>
+      <c r="F173" s="5">
+        <v>2</v>
+      </c>
       <c r="G173" s="5"/>
     </row>
-    <row r="174" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="8"/>
       <c r="B174" s="11" t="s">
         <v>86</v>
@@ -3851,10 +4061,12 @@
         <v>4</v>
       </c>
       <c r="E174" s="5"/>
-      <c r="F174" s="5"/>
+      <c r="F174" s="5">
+        <v>2</v>
+      </c>
       <c r="G174" s="5"/>
     </row>
-    <row r="175" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="B175" s="11"/>
       <c r="C175" s="5"/>
@@ -3863,26 +4075,44 @@
         <v>2512</v>
       </c>
       <c r="E175" s="7">
-        <f>SUM(E2:E174)</f>
-        <v>104</v>
+        <f>D175-(F175+G175)</f>
+        <v>510</v>
       </c>
       <c r="F175" s="7">
         <f>SUM(F2:F174)</f>
-        <v>708</v>
+        <v>1220</v>
       </c>
       <c r="G175" s="7">
         <f>SUM(G2:G174)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>782</v>
+      </c>
+      <c r="H175" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="B176" s="11"/>
       <c r="C176" s="5"/>
-      <c r="D176" s="5"/>
-      <c r="E176" s="5"/>
-      <c r="F176" s="5"/>
-      <c r="G176" s="5"/>
+      <c r="D176" s="5">
+        <f>D175/8</f>
+        <v>314</v>
+      </c>
+      <c r="E176" s="5">
+        <f>E175/8</f>
+        <v>63.75</v>
+      </c>
+      <c r="F176" s="5">
+        <f>F175/8</f>
+        <v>152.5</v>
+      </c>
+      <c r="G176" s="5">
+        <f>G175/8</f>
+        <v>97.75</v>
+      </c>
+      <c r="H176" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="177" spans="1:7" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>

</xml_diff>